<commit_message>
18.10.2024 - ok el color naranja
</commit_message>
<xml_diff>
--- a/resultado_colores.xlsx
+++ b/resultado_colores.xlsx
@@ -487,7 +487,7 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -526,7 +526,7 @@
         <v>14</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -630,7 +630,7 @@
         <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -643,7 +643,7 @@
         <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -669,7 +669,7 @@
         <v>0</v>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20">
@@ -695,7 +695,7 @@
         <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22">
@@ -708,7 +708,7 @@
         <v>0</v>
       </c>
       <c r="C22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
@@ -721,7 +721,7 @@
         <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
@@ -734,7 +734,7 @@
         <v>0</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
@@ -760,7 +760,7 @@
         <v>1</v>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27">
@@ -799,7 +799,7 @@
         <v>0</v>
       </c>
       <c r="C29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
@@ -812,7 +812,7 @@
         <v>38</v>
       </c>
       <c r="C30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
@@ -825,7 +825,7 @@
         <v>0</v>
       </c>
       <c r="C31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
@@ -838,7 +838,7 @@
         <v>0</v>
       </c>
       <c r="C32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
@@ -851,7 +851,7 @@
         <v>0</v>
       </c>
       <c r="C33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
@@ -864,7 +864,7 @@
         <v>0</v>
       </c>
       <c r="C34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
@@ -877,7 +877,7 @@
         <v>0</v>
       </c>
       <c r="C35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36">
@@ -890,7 +890,7 @@
         <v>0</v>
       </c>
       <c r="C36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37">
@@ -903,7 +903,7 @@
         <v>0</v>
       </c>
       <c r="C37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
@@ -916,7 +916,7 @@
         <v>0</v>
       </c>
       <c r="C38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
@@ -929,7 +929,7 @@
         <v>0</v>
       </c>
       <c r="C39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40">
@@ -942,7 +942,7 @@
         <v>0</v>
       </c>
       <c r="C40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
@@ -955,7 +955,7 @@
         <v>0</v>
       </c>
       <c r="C41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
@@ -968,7 +968,7 @@
         <v>0</v>
       </c>
       <c r="C42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43">
@@ -981,7 +981,7 @@
         <v>0</v>
       </c>
       <c r="C43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44">
@@ -994,7 +994,7 @@
         <v>0</v>
       </c>
       <c r="C44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
@@ -1007,7 +1007,7 @@
         <v>0</v>
       </c>
       <c r="C45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46">
@@ -1020,7 +1020,7 @@
         <v>0</v>
       </c>
       <c r="C46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47">
@@ -1033,7 +1033,7 @@
         <v>0</v>
       </c>
       <c r="C47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48">
@@ -1046,7 +1046,7 @@
         <v>0</v>
       </c>
       <c r="C48" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49">
@@ -1059,7 +1059,7 @@
         <v>0</v>
       </c>
       <c r="C49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50">
@@ -1072,7 +1072,7 @@
         <v>0</v>
       </c>
       <c r="C50" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51">
@@ -1137,7 +1137,7 @@
         <v>21</v>
       </c>
       <c r="C55" t="n">
-        <v>0</v>
+        <v>47</v>
       </c>
     </row>
     <row r="56">
@@ -1150,7 +1150,7 @@
         <v>0</v>
       </c>
       <c r="C56" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57">

</xml_diff>

<commit_message>
18.10.2024- Ok color naranja y total de columna roja y naranja
</commit_message>
<xml_diff>
--- a/resultado_colores.xlsx
+++ b/resultado_colores.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C59"/>
+  <dimension ref="A1:C60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1192,6 +1192,19 @@
         <v>0</v>
       </c>
     </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>158</v>
+      </c>
+      <c r="C60" t="n">
+        <v>111</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
24.10.2024 - ok colores y contar
</commit_message>
<xml_diff>
--- a/resultado_colores.xlsx
+++ b/resultado_colores.xlsx
@@ -487,7 +487,7 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -526,7 +526,7 @@
         <v>14</v>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -630,7 +630,7 @@
         <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -643,7 +643,7 @@
         <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -708,7 +708,7 @@
         <v>0</v>
       </c>
       <c r="C22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -721,7 +721,7 @@
         <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -734,7 +734,7 @@
         <v>0</v>
       </c>
       <c r="C24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -799,7 +799,7 @@
         <v>0</v>
       </c>
       <c r="C29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -812,7 +812,7 @@
         <v>38</v>
       </c>
       <c r="C30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -825,7 +825,7 @@
         <v>0</v>
       </c>
       <c r="C31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -838,7 +838,7 @@
         <v>0</v>
       </c>
       <c r="C32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -851,7 +851,7 @@
         <v>0</v>
       </c>
       <c r="C33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -864,7 +864,7 @@
         <v>0</v>
       </c>
       <c r="C34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -877,7 +877,7 @@
         <v>0</v>
       </c>
       <c r="C35" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36">
@@ -890,7 +890,7 @@
         <v>0</v>
       </c>
       <c r="C36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -903,7 +903,7 @@
         <v>0</v>
       </c>
       <c r="C37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -916,7 +916,7 @@
         <v>0</v>
       </c>
       <c r="C38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -929,7 +929,7 @@
         <v>0</v>
       </c>
       <c r="C39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -942,7 +942,7 @@
         <v>0</v>
       </c>
       <c r="C40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -955,7 +955,7 @@
         <v>0</v>
       </c>
       <c r="C41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -968,7 +968,7 @@
         <v>0</v>
       </c>
       <c r="C42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -981,7 +981,7 @@
         <v>0</v>
       </c>
       <c r="C43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -994,7 +994,7 @@
         <v>0</v>
       </c>
       <c r="C44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -1007,7 +1007,7 @@
         <v>0</v>
       </c>
       <c r="C45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -1020,7 +1020,7 @@
         <v>0</v>
       </c>
       <c r="C46" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47">
@@ -1033,7 +1033,7 @@
         <v>0</v>
       </c>
       <c r="C47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -1059,7 +1059,7 @@
         <v>0</v>
       </c>
       <c r="C49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -1072,7 +1072,7 @@
         <v>0</v>
       </c>
       <c r="C50" t="n">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="51">
@@ -1202,7 +1202,7 @@
         <v>158</v>
       </c>
       <c r="C60" t="n">
-        <v>111</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>